<commit_message>
Se hizo un piloto
Aun falta arregalr orden y lista de modelos
</commit_message>
<xml_diff>
--- a/Formato 1/ilm_Scrap.xlsx
+++ b/Formato 1/ilm_Scrap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
   <si>
     <t>list name</t>
   </si>
@@ -202,21 +202,6 @@
   </si>
   <si>
     <t>Colocar correctamente el peso</t>
-  </si>
-  <si>
-    <t>${Peso1}</t>
-  </si>
-  <si>
-    <t>${Peso2}</t>
-  </si>
-  <si>
-    <t>${Peso3}</t>
-  </si>
-  <si>
-    <t>${Peso4}</t>
-  </si>
-  <si>
-    <t>${Peso5}</t>
   </si>
   <si>
     <t>Algun Posible Comentario</t>
@@ -739,7 +724,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -749,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -946,9 +931,7 @@
         <v>42</v>
       </c>
       <c r="G7" s="28"/>
-      <c r="H7" s="28" t="s">
-        <v>62</v>
-      </c>
+      <c r="H7" s="28"/>
       <c r="I7" s="28"/>
       <c r="J7" s="28" t="s">
         <v>26</v>
@@ -976,9 +959,7 @@
         <v>42</v>
       </c>
       <c r="G8" s="28"/>
-      <c r="H8" s="28" t="s">
-        <v>63</v>
-      </c>
+      <c r="H8" s="28"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28" t="s">
         <v>26</v>
@@ -1006,9 +987,7 @@
         <v>42</v>
       </c>
       <c r="G9" s="28"/>
-      <c r="H9" s="28" t="s">
-        <v>64</v>
-      </c>
+      <c r="H9" s="28"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28" t="s">
         <v>26</v>
@@ -1036,9 +1015,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="28"/>
-      <c r="H10" s="28" t="s">
-        <v>66</v>
-      </c>
+      <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28" t="s">
         <v>26</v>
@@ -1066,9 +1043,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="28"/>
-      <c r="H11" s="28" t="s">
-        <v>65</v>
-      </c>
+      <c r="H11" s="28"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28" t="s">
         <v>26</v>
@@ -1084,7 +1059,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>30</v>
@@ -1108,7 +1083,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>41</v>
@@ -1205,7 +1180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D573"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11:C32"/>
     </sheetView>
   </sheetViews>
@@ -1238,7 +1213,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>33</v>
@@ -1250,7 +1225,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>34</v>
@@ -1262,7 +1237,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>35</v>
@@ -1274,10 +1249,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>78</v>
       </c>
       <c r="D5" s="19"/>
     </row>
@@ -1286,10 +1261,10 @@
         <v>44</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>79</v>
       </c>
       <c r="D6" s="19"/>
     </row>
@@ -1298,10 +1273,10 @@
         <v>44</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>80</v>
       </c>
       <c r="D7" s="19"/>
     </row>
@@ -1310,10 +1285,10 @@
         <v>44</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>76</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>81</v>
       </c>
       <c r="D8" s="19"/>
     </row>
@@ -1322,10 +1297,10 @@
         <v>44</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>77</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>82</v>
       </c>
       <c r="D9" s="17"/>
     </row>
@@ -4515,7 +4490,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>40</v>

</xml_diff>